<commit_message>
cleaned data for a more polished format for analysis
</commit_message>
<xml_diff>
--- a/Data_Sets/nfl_stadiums.xlsx
+++ b/Data_Sets/nfl_stadiums.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynnpowell/Documents/DS_Projects/NFL_Analysis/Data_Sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DD808C-D09D-5B4C-B95F-E43C2081890E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA67FC3-8AFC-B643-A49C-7D97E135E0D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47960" yWindow="820" windowWidth="15900" windowHeight="16680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -352,15 +352,6 @@
     <t>Retractable</t>
   </si>
   <si>
-    <t>Reputation</t>
-  </si>
-  <si>
-    <t>Loud Fans</t>
-  </si>
-  <si>
-    <t>Altitude</t>
-  </si>
-  <si>
     <t>Weather</t>
   </si>
   <si>
@@ -431,6 +422,9 @@
   </si>
   <si>
     <t>NFC South</t>
+  </si>
+  <si>
+    <t>Fan_Repu</t>
   </si>
 </sst>
 </file>
@@ -788,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -827,19 +821,19 @@
         <v>106</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -864,17 +858,20 @@
       <c r="G2" t="s">
         <v>107</v>
       </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
       <c r="I2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -896,17 +893,20 @@
       <c r="G3" t="s">
         <v>108</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K3" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" t="s">
         <v>128</v>
-      </c>
-      <c r="L3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -931,20 +931,20 @@
       <c r="G4" t="s">
         <v>107</v>
       </c>
-      <c r="H4" t="s">
-        <v>111</v>
+      <c r="H4">
+        <v>1</v>
       </c>
       <c r="I4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" t="s">
         <v>116</v>
       </c>
-      <c r="J4" t="s">
-        <v>119</v>
-      </c>
       <c r="K4" t="s">
+        <v>125</v>
+      </c>
+      <c r="L4" t="s">
         <v>128</v>
-      </c>
-      <c r="L4" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -966,17 +966,20 @@
       <c r="G5" t="s">
         <v>109</v>
       </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
       <c r="I5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -998,17 +1001,20 @@
       <c r="G6" t="s">
         <v>107</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
       <c r="I6" t="s">
+        <v>113</v>
+      </c>
+      <c r="J6" t="s">
         <v>116</v>
       </c>
-      <c r="J6" t="s">
-        <v>119</v>
-      </c>
       <c r="K6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1033,20 +1039,20 @@
       <c r="G7" t="s">
         <v>107</v>
       </c>
-      <c r="H7" t="s">
-        <v>112</v>
+      <c r="H7">
+        <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K7" t="s">
+        <v>125</v>
+      </c>
+      <c r="L7" t="s">
         <v>128</v>
-      </c>
-      <c r="L7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1068,17 +1074,20 @@
       <c r="G8" t="s">
         <v>107</v>
       </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="I8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J8" t="s">
         <v>116</v>
       </c>
-      <c r="J8" t="s">
-        <v>119</v>
-      </c>
       <c r="K8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1103,17 +1112,20 @@
       <c r="G9" t="s">
         <v>107</v>
       </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
       <c r="I9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1135,17 +1147,20 @@
       <c r="G10" t="s">
         <v>108</v>
       </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
       <c r="I10" t="s">
+        <v>112</v>
+      </c>
+      <c r="J10" t="s">
         <v>115</v>
       </c>
-      <c r="J10" t="s">
-        <v>118</v>
-      </c>
       <c r="K10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1170,20 +1185,20 @@
       <c r="G11" t="s">
         <v>107</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
         <v>111</v>
       </c>
-      <c r="I11" t="s">
-        <v>114</v>
-      </c>
       <c r="J11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1205,17 +1220,20 @@
       <c r="G12" t="s">
         <v>107</v>
       </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
       <c r="I12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J12" t="s">
+        <v>117</v>
+      </c>
+      <c r="K12" t="s">
         <v>120</v>
       </c>
-      <c r="K12" t="s">
-        <v>123</v>
-      </c>
       <c r="L12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1237,17 +1255,20 @@
       <c r="G13" t="s">
         <v>107</v>
       </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
       <c r="I13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1269,20 +1290,20 @@
       <c r="G14" t="s">
         <v>107</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
         <v>111</v>
       </c>
-      <c r="I14" t="s">
-        <v>114</v>
-      </c>
       <c r="J14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1304,17 +1325,20 @@
       <c r="G15" t="s">
         <v>107</v>
       </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
       <c r="I15" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" t="s">
         <v>116</v>
       </c>
-      <c r="J15" t="s">
-        <v>119</v>
-      </c>
       <c r="K15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1339,20 +1363,20 @@
       <c r="G16" t="s">
         <v>107</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
         <v>111</v>
       </c>
-      <c r="I16" t="s">
-        <v>114</v>
-      </c>
       <c r="J16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1377,17 +1401,20 @@
       <c r="G17" t="s">
         <v>109</v>
       </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
       <c r="I17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1409,20 +1436,20 @@
       <c r="G18" t="s">
         <v>107</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
         <v>111</v>
       </c>
-      <c r="I18" t="s">
-        <v>114</v>
-      </c>
       <c r="J18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1447,17 +1474,20 @@
       <c r="G19" t="s">
         <v>107</v>
       </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
       <c r="I19" t="s">
+        <v>113</v>
+      </c>
+      <c r="J19" t="s">
         <v>116</v>
       </c>
-      <c r="J19" t="s">
-        <v>119</v>
-      </c>
       <c r="K19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L19" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1479,20 +1509,20 @@
       <c r="G20" t="s">
         <v>109</v>
       </c>
-      <c r="H20" t="s">
-        <v>111</v>
+      <c r="H20">
+        <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1500,7 +1530,7 @@
         <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C21" s="2">
         <v>82500</v>
@@ -1517,17 +1547,20 @@
       <c r="G21" t="s">
         <v>107</v>
       </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
       <c r="I21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K21" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1552,17 +1585,20 @@
       <c r="G22" t="s">
         <v>107</v>
       </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
       <c r="I22" t="s">
+        <v>113</v>
+      </c>
+      <c r="J22" t="s">
         <v>116</v>
       </c>
-      <c r="J22" t="s">
-        <v>119</v>
-      </c>
       <c r="K22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1587,17 +1623,20 @@
       <c r="G23" t="s">
         <v>109</v>
       </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
       <c r="I23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L23" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1622,17 +1661,20 @@
       <c r="G24" t="s">
         <v>107</v>
       </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
       <c r="I24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J24" t="s">
         <v>116</v>
       </c>
-      <c r="J24" t="s">
-        <v>119</v>
-      </c>
       <c r="K24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1654,17 +1696,20 @@
       <c r="G25" t="s">
         <v>107</v>
       </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
       <c r="I25" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K25" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -1672,7 +1717,7 @@
         <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C26" s="2">
         <v>70000</v>
@@ -1686,17 +1731,20 @@
       <c r="G26" t="s">
         <v>108</v>
       </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
       <c r="I26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -1718,20 +1766,20 @@
       <c r="G27" t="s">
         <v>107</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
         <v>111</v>
       </c>
-      <c r="I27" t="s">
-        <v>114</v>
-      </c>
       <c r="J27" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -1753,20 +1801,20 @@
       <c r="G28" t="s">
         <v>108</v>
       </c>
-      <c r="H28" t="s">
-        <v>111</v>
+      <c r="H28">
+        <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J28" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -1788,17 +1836,20 @@
       <c r="G29" t="s">
         <v>107</v>
       </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
       <c r="I29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J29" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K29" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -1823,17 +1874,20 @@
       <c r="G30" t="s">
         <v>109</v>
       </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
       <c r="I30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J30" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -1855,20 +1909,20 @@
       <c r="G31" t="s">
         <v>108</v>
       </c>
-      <c r="H31" t="s">
-        <v>111</v>
+      <c r="H31">
+        <v>1</v>
       </c>
       <c r="I31" t="s">
+        <v>112</v>
+      </c>
+      <c r="J31" t="s">
         <v>115</v>
       </c>
-      <c r="J31" t="s">
-        <v>118</v>
-      </c>
       <c r="K31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -1876,7 +1930,7 @@
         <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C32" s="2">
         <v>82500</v>
@@ -1893,17 +1947,20 @@
       <c r="G32" t="s">
         <v>107</v>
       </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
       <c r="I32" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J32" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K32" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L32" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -1911,7 +1968,7 @@
         <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C33" s="2">
         <v>70000</v>
@@ -1925,17 +1982,20 @@
       <c r="G33" t="s">
         <v>108</v>
       </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
       <c r="I33" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K33" t="s">
+        <v>125</v>
+      </c>
+      <c r="L33" t="s">
         <v>128</v>
-      </c>
-      <c r="L33" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>